<commit_message>
zname chyby v zadavani planu jsou odstraneny
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\maxu\finegusto_plan\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mokry\Desktop\Finegusto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D5F3C0-DD5D-4FBE-BDA8-0A0A811E4F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE45492E-4DAC-4E59-ABF3-0A0CCFBEABEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43BB1CFA-D819-4C4C-91AC-73CB590F3D68}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{43BB1CFA-D819-4C4C-91AC-73CB590F3D68}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,42 +474,27 @@
         <v>394</v>
       </c>
       <c r="D2" s="3">
-        <v>1000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
-        <v>45889</v>
+        <v>45890</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D3" s="3">
-        <v>1000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>45890</v>
-      </c>
-      <c r="C4">
-        <v>394</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>45890</v>
-      </c>
-      <c r="C5" s="3">
-        <v>395</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hotova druha funkiconalita, pridany testy
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mokry\Desktop\Finegusto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE45492E-4DAC-4E59-ABF3-0A0CCFBEABEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7BF67C-44F6-4E91-974E-314ED5FB8FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{43BB1CFA-D819-4C4C-91AC-73CB590F3D68}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43BB1CFA-D819-4C4C-91AC-73CB590F3D68}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>datum</t>
-  </si>
-  <si>
-    <t>vyrobek</t>
   </si>
   <si>
     <t>mnozstvi</t>
@@ -93,7 +90,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -104,7 +101,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -439,62 +435,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DA80B1-4108-4CBB-B24D-7A3E4FADACF3}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45889</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="3">
+        <v>394</v>
+      </c>
       <c r="C2" s="3">
-        <v>394</v>
-      </c>
-      <c r="D2" s="3">
         <v>4000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45890</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>394</v>
+      </c>
       <c r="C3" s="3">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45892</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45892</v>
+      </c>
+      <c r="B5" s="3">
+        <v>102</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45897</v>
+      </c>
+      <c r="B6" s="3">
         <v>394</v>
       </c>
-      <c r="D3" s="3">
+      <c r="C6" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45897</v>
+      </c>
+      <c r="B7" s="3">
+        <v>394</v>
+      </c>
+      <c r="C7" s="3">
         <v>8000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="C5" s="3"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45897</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45899</v>
+      </c>
+      <c r="B9" s="3">
+        <v>102</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>